<commit_message>
Add code auth v2
</commit_message>
<xml_diff>
--- a/document/NRM APISpecs.xlsx
+++ b/document/NRM APISpecs.xlsx
@@ -682,7 +682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -806,6 +806,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1124,7 +1128,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="A2:F2"/>
+      <selection activeCell="A3" sqref="A3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,32 +1176,32 @@
       <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="44" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="44"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="54"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
@@ -1270,20 +1274,20 @@
       <c r="F9" s="48"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="44" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="48"/>
+      <c r="F10" s="54"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="45"/>
@@ -3288,7 +3292,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3476,7 +3480,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3699,7 +3703,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add code login and create account.
</commit_message>
<xml_diff>
--- a/document/NRM APISpecs.xlsx
+++ b/document/NRM APISpecs.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="133">
   <si>
     <t>No.</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>A reason</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -677,12 +680,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -810,6 +822,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1125,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,7 +1154,7 @@
     <col min="6" max="6" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="50"/>
       <c r="B2" s="43" t="s">
         <v>6</v>
@@ -1175,7 +1188,7 @@
       <c r="E2" s="52"/>
       <c r="F2" s="43"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="50"/>
       <c r="B3" s="43" t="s">
         <v>9</v>
@@ -1189,7 +1202,7 @@
       <c r="E3" s="52"/>
       <c r="F3" s="43"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
       <c r="B4" s="43" t="s">
         <v>11</v>
@@ -1203,21 +1216,22 @@
       <c r="E4" s="52"/>
       <c r="F4" s="54"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
-      <c r="B5" s="44" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="50"/>
+      <c r="B5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="52"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="44" t="s">
         <v>15</v>
@@ -1231,7 +1245,7 @@
       <c r="E6" s="47"/>
       <c r="F6" s="48"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="44" t="s">
         <v>17</v>
@@ -1245,7 +1259,7 @@
       <c r="E7" s="47"/>
       <c r="F7" s="48"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
       <c r="B8" s="44" t="s">
         <v>19</v>
@@ -1259,7 +1273,7 @@
       <c r="E8" s="47"/>
       <c r="F8" s="48"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
       <c r="B9" s="44" t="s">
         <v>21</v>
@@ -1272,8 +1286,11 @@
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="48"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
       <c r="B10" s="43" t="s">
         <v>24</v>
@@ -1289,23 +1306,23 @@
       </c>
       <c r="F10" s="54"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="44" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="50"/>
+      <c r="B11" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="48"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="54"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="1" t="s">
         <v>29</v>
@@ -1321,7 +1338,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="1" t="s">
         <v>31</v>
@@ -1337,7 +1354,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="1" t="s">
         <v>33</v>
@@ -1355,7 +1372,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="1" t="s">
         <v>36</v>
@@ -1371,7 +1388,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="1" t="s">
         <v>38</v>
@@ -1826,7 +1843,7 @@
   <dimension ref="B2:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,7 +2682,7 @@
   <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,7 +3497,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3703,7 +3720,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add auth login v3
</commit_message>
<xml_diff>
--- a/document/NRM APISpecs.xlsx
+++ b/document/NRM APISpecs.xlsx
@@ -15,12 +15,12 @@
     <sheet name="List API" sheetId="2" r:id="rId1"/>
     <sheet name="signIn" sheetId="5" r:id="rId2"/>
     <sheet name="getAccount" sheetId="10" r:id="rId3"/>
-    <sheet name="refreshCredentials" sheetId="9" r:id="rId4"/>
-    <sheet name="signUpValidateEmail" sheetId="14" r:id="rId5"/>
-    <sheet name="signUp" sheetId="4" r:id="rId6"/>
-    <sheet name="signUpConfirm" sheetId="3" r:id="rId7"/>
-    <sheet name="forgotPasswordInitiate" sheetId="6" r:id="rId8"/>
-    <sheet name="forgotPasswordInitiateEmail" sheetId="7" r:id="rId9"/>
+    <sheet name="forgotPasswordInitiate" sheetId="6" r:id="rId4"/>
+    <sheet name="forgotPasswordInitiateEmail" sheetId="7" r:id="rId5"/>
+    <sheet name="refreshCredentials" sheetId="9" r:id="rId6"/>
+    <sheet name="signUpValidateEmail" sheetId="14" r:id="rId7"/>
+    <sheet name="signUp" sheetId="4" r:id="rId8"/>
+    <sheet name="signUpConfirm" sheetId="3" r:id="rId9"/>
     <sheet name="forgotPasswordChange" sheetId="8" r:id="rId10"/>
     <sheet name="updateAccount" sheetId="11" r:id="rId11"/>
     <sheet name="changePassword" sheetId="12" r:id="rId12"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="132">
   <si>
     <t>No.</t>
   </si>
@@ -541,9 +541,6 @@
   </si>
   <si>
     <t>A reason</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -694,7 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -808,9 +805,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1141,7 +1135,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,61 +1169,61 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
+      <c r="A2" s="49"/>
       <c r="B2" s="43" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="52"/>
+      <c r="E2" s="51"/>
       <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="43" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="52"/>
+      <c r="E3" s="51"/>
       <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="43" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="54"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="53"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="43" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="55"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
@@ -1274,53 +1268,50 @@
       <c r="F8" s="48"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="44" t="s">
+      <c r="A9" s="49"/>
+      <c r="B9" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="49"/>
-      <c r="F9" s="48"/>
-      <c r="G9" t="s">
-        <v>132</v>
-      </c>
+      <c r="E9" s="52"/>
+      <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="43" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="54"/>
+      <c r="F10" s="53"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="43" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="53" t="s">
+      <c r="E11" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="54"/>
+      <c r="F11" s="53"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -1843,7 +1834,7 @@
   <dimension ref="B2:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2918,8 +2909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,7 +3120,382 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="13">
+        <v>200</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="13">
+        <v>400</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="13">
+        <v>404</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="27"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="28"/>
+      <c r="D14" s="39"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="13">
+        <v>200</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="13">
+        <v>400</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="13">
+        <v>404</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="27"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="28"/>
+      <c r="D14" s="39"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3304,7 +3670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G14"/>
   <sheetViews>
@@ -3492,12 +3858,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3715,7 +4081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
@@ -3932,379 +4298,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="13">
-        <v>200</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="13">
-        <v>400</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="13">
-        <v>404</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="27"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="28"/>
-      <c r="D14" s="39"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="13">
-        <v>200</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="13">
-        <v>400</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="13">
-        <v>404</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="27"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="28"/>
-      <c r="D14" s="39"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="F8" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add code forgotPasswordInitiate and forgotPasswordInitiateEmail
</commit_message>
<xml_diff>
--- a/document/NRM APISpecs.xlsx
+++ b/document/NRM APISpecs.xlsx
@@ -22,8 +22,8 @@
     <sheet name="signUp" sheetId="4" r:id="rId8"/>
     <sheet name="signUpConfirm" sheetId="3" r:id="rId9"/>
     <sheet name="forgotPasswordChange" sheetId="8" r:id="rId10"/>
-    <sheet name="updateAccount" sheetId="11" r:id="rId11"/>
-    <sheet name="changePassword" sheetId="12" r:id="rId12"/>
+    <sheet name="changePassword" sheetId="12" r:id="rId11"/>
+    <sheet name="updateAccount" sheetId="11" r:id="rId12"/>
     <sheet name="terminateAccount" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,32 +1226,32 @@
       <c r="G5" s="54"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="44" t="s">
+      <c r="A6" s="49"/>
+      <c r="B6" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="48"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="44" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="48"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="53"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
@@ -1599,6 +1599,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1607,7 +1608,7 @@
   <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,407 +1831,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-    </row>
-    <row r="24" spans="2:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
-      <c r="C24" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="41">
-        <v>200</v>
-      </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="13">
-        <v>400</v>
-      </c>
-      <c r="E25" s="23"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="13">
-        <v>403</v>
-      </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="D27" s="13">
-        <v>400</v>
-      </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="28"/>
-      <c r="D28" s="39"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="F11" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G16"/>
   <sheetViews>
@@ -2457,12 +2057,413 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="24"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="2:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="41">
+        <v>200</v>
+      </c>
+      <c r="E24" s="30"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="13">
+        <v>400</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="13">
+        <v>403</v>
+      </c>
+      <c r="E26" s="23"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="13">
+        <v>400</v>
+      </c>
+      <c r="E27" s="23"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="28"/>
+      <c r="D28" s="39"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F11" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3120,7 +3121,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3307,7 +3308,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,7 +3496,7 @@
   <dimension ref="B2:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>